<commit_message>
added fuel use and cost in addition to fuel remaining
</commit_message>
<xml_diff>
--- a/planning_info/NE_chartering_2021_Aug_Borek.xlsx
+++ b/planning_info/NE_chartering_2021_Aug_Borek.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V19"/>
+  <dimension ref="A1:W19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,50 +497,55 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
+          <t>fuel_remaining(liters)</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
           <t>arrival time (local time)</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>stoppage time (h)</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>from lat</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>from lon</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>destination lat</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>destination lon</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>start location name</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>landing location name</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>air speed kt</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>description of work</t>
         </is>
@@ -594,39 +599,42 @@
         <v>14</v>
       </c>
       <c r="M2" t="n">
+        <v>9</v>
+      </c>
+      <c r="N2" t="n">
         <v>12.1</v>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>end of flying</t>
         </is>
       </c>
-      <c r="O2" t="n">
+      <c r="P2" t="n">
         <v>63.7553</v>
       </c>
-      <c r="P2" t="n">
+      <c r="Q2" t="n">
         <v>-68.5506</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="R2" t="n">
         <v>67.0106</v>
       </c>
-      <c r="R2" t="n">
+      <c r="S2" t="n">
         <v>-50.711</v>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>Iqaluit</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="U2" t="inlineStr">
         <is>
           <t>Kangerlussuaq</t>
         </is>
       </c>
-      <c r="U2" t="n">
+      <c r="V2" t="n">
         <v>140</v>
       </c>
-      <c r="V2" t="inlineStr">
+      <c r="W2" t="inlineStr">
         <is>
           <t>transit from Iqaluit with no cargo</t>
         </is>
@@ -661,6 +669,7 @@
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -710,41 +719,44 @@
         <v>12</v>
       </c>
       <c r="M4" t="n">
+        <v>202</v>
+      </c>
+      <c r="N4" t="n">
         <v>11.4</v>
       </c>
-      <c r="N4" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="O4" t="n">
+      <c r="P4" t="n">
         <v>67.0106</v>
       </c>
-      <c r="P4" t="n">
+      <c r="Q4" t="n">
         <v>-50.711</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="R4" t="n">
         <v>72.5797</v>
       </c>
-      <c r="R4" t="n">
+      <c r="S4" t="n">
         <v>-38.5045</v>
       </c>
-      <c r="S4" t="inlineStr">
+      <c r="T4" t="inlineStr">
         <is>
           <t>Kangerlussuaq</t>
         </is>
       </c>
-      <c r="T4" t="inlineStr">
+      <c r="U4" t="inlineStr">
         <is>
           <t>Summit</t>
         </is>
       </c>
-      <c r="U4" t="n">
+      <c r="V4" t="n">
         <v>140</v>
       </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>refuel at Summit. basic maintanance at Summit</t>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>refuel at Summit 2 x 200 liters. basic maintanance at Summit</t>
         </is>
       </c>
     </row>
@@ -796,39 +808,42 @@
         <v>30</v>
       </c>
       <c r="M5" t="n">
+        <v>65</v>
+      </c>
+      <c r="N5" t="n">
         <v>17.1</v>
       </c>
-      <c r="N5" t="inlineStr">
+      <c r="O5" t="inlineStr">
         <is>
           <t>end of flying</t>
         </is>
       </c>
-      <c r="O5" t="n">
+      <c r="P5" t="n">
         <v>72.5797</v>
       </c>
-      <c r="P5" t="n">
+      <c r="Q5" t="n">
         <v>-38.5045</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="R5" t="n">
         <v>75.62479999999999</v>
       </c>
-      <c r="R5" t="n">
+      <c r="S5" t="n">
         <v>-35.9729</v>
       </c>
-      <c r="S5" t="inlineStr">
+      <c r="T5" t="inlineStr">
         <is>
           <t>Summit</t>
         </is>
       </c>
-      <c r="T5" t="inlineStr">
+      <c r="U5" t="inlineStr">
         <is>
           <t>EGP</t>
         </is>
       </c>
-      <c r="U5" t="n">
+      <c r="V5" t="n">
         <v>140</v>
       </c>
-      <c r="V5" t="inlineStr">
+      <c r="W5" t="inlineStr">
         <is>
           <t>EGP new AWS install. Twin Otter overnights</t>
         </is>
@@ -863,6 +878,7 @@
       <c r="T6" t="inlineStr"/>
       <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -891,6 +907,7 @@
       <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -940,39 +957,42 @@
         <v>3</v>
       </c>
       <c r="M8" t="n">
+        <v>1118</v>
+      </c>
+      <c r="N8" t="n">
         <v>10.1</v>
       </c>
-      <c r="N8" t="inlineStr">
+      <c r="O8" t="inlineStr">
         <is>
           <t>4.0</t>
         </is>
       </c>
-      <c r="O8" t="n">
+      <c r="P8" t="n">
         <v>75.62479999999999</v>
       </c>
-      <c r="P8" t="n">
+      <c r="Q8" t="n">
         <v>-35.9729</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="R8" t="n">
         <v>75</v>
       </c>
-      <c r="R8" t="n">
+      <c r="S8" t="n">
         <v>-29.9997</v>
       </c>
-      <c r="S8" t="inlineStr">
+      <c r="T8" t="inlineStr">
         <is>
           <t>EGP</t>
         </is>
       </c>
-      <c r="T8" t="inlineStr">
+      <c r="U8" t="inlineStr">
         <is>
           <t>NASA-E</t>
         </is>
       </c>
-      <c r="U8" t="n">
+      <c r="V8" t="n">
         <v>140</v>
       </c>
-      <c r="V8" t="inlineStr">
+      <c r="W8" t="inlineStr">
         <is>
           <t>maintanance at NASA-E</t>
         </is>
@@ -1026,39 +1046,42 @@
         <v>9</v>
       </c>
       <c r="M9" t="n">
+        <v>836</v>
+      </c>
+      <c r="N9" t="n">
         <v>15.2</v>
       </c>
-      <c r="N9" t="inlineStr">
+      <c r="O9" t="inlineStr">
         <is>
           <t>4.0</t>
         </is>
       </c>
-      <c r="O9" t="n">
+      <c r="P9" t="n">
         <v>75</v>
       </c>
-      <c r="P9" t="n">
+      <c r="Q9" t="n">
         <v>-29.9997</v>
       </c>
-      <c r="Q9" t="n">
+      <c r="R9" t="n">
         <v>75.62479999999999</v>
       </c>
-      <c r="R9" t="n">
+      <c r="S9" t="n">
         <v>-35.9729</v>
       </c>
-      <c r="S9" t="inlineStr">
+      <c r="T9" t="inlineStr">
         <is>
           <t>NASA-E</t>
         </is>
       </c>
-      <c r="T9" t="inlineStr">
+      <c r="U9" t="inlineStr">
         <is>
           <t>EGP</t>
         </is>
       </c>
-      <c r="U9" t="n">
+      <c r="V9" t="n">
         <v>140</v>
       </c>
-      <c r="V9" t="inlineStr">
+      <c r="W9" t="inlineStr">
         <is>
           <t>return to EGP for overnight 2</t>
         </is>
@@ -1093,6 +1116,7 @@
       <c r="T10" t="inlineStr"/>
       <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1142,39 +1166,42 @@
         <v>7</v>
       </c>
       <c r="M11" t="n">
+        <v>716</v>
+      </c>
+      <c r="N11" t="n">
         <v>11.1</v>
       </c>
-      <c r="N11" t="inlineStr">
+      <c r="O11" t="inlineStr">
         <is>
           <t>4.0</t>
         </is>
       </c>
-      <c r="O11" t="n">
+      <c r="P11" t="n">
         <v>75.62479999999999</v>
       </c>
-      <c r="P11" t="n">
+      <c r="Q11" t="n">
         <v>-35.9729</v>
       </c>
-      <c r="Q11" t="n">
+      <c r="R11" t="n">
         <v>73.8419</v>
       </c>
-      <c r="R11" t="n">
+      <c r="S11" t="n">
         <v>-49.4983</v>
       </c>
-      <c r="S11" t="inlineStr">
+      <c r="T11" t="inlineStr">
         <is>
           <t>EGP</t>
         </is>
       </c>
-      <c r="T11" t="inlineStr">
+      <c r="U11" t="inlineStr">
         <is>
           <t>NASA-U</t>
         </is>
       </c>
-      <c r="U11" t="n">
+      <c r="V11" t="n">
         <v>140</v>
       </c>
-      <c r="V11" t="inlineStr">
+      <c r="W11" t="inlineStr">
         <is>
           <t>crane maintanance at NASA-U</t>
         </is>
@@ -1228,39 +1255,42 @@
         <v>18</v>
       </c>
       <c r="M12" t="n">
+        <v>342</v>
+      </c>
+      <c r="N12" t="n">
         <v>16.4</v>
       </c>
-      <c r="N12" t="inlineStr">
+      <c r="O12" t="inlineStr">
         <is>
           <t>end of flying</t>
         </is>
       </c>
-      <c r="O12" t="n">
+      <c r="P12" t="n">
         <v>73.8419</v>
       </c>
-      <c r="P12" t="n">
+      <c r="Q12" t="n">
         <v>-49.4983</v>
       </c>
-      <c r="Q12" t="n">
+      <c r="R12" t="n">
         <v>72.79000000000001</v>
       </c>
-      <c r="R12" t="n">
+      <c r="S12" t="n">
         <v>-56.1305</v>
       </c>
-      <c r="S12" t="inlineStr">
+      <c r="T12" t="inlineStr">
         <is>
           <t>NASA-U</t>
         </is>
       </c>
-      <c r="T12" t="inlineStr">
+      <c r="U12" t="inlineStr">
         <is>
           <t>Upernavik</t>
         </is>
       </c>
-      <c r="U12" t="n">
+      <c r="V12" t="n">
         <v>140</v>
       </c>
-      <c r="V12" t="inlineStr">
+      <c r="W12" t="inlineStr">
         <is>
           <t>return to coast. Upernavik</t>
         </is>
@@ -1295,6 +1325,7 @@
       <c r="T13" t="inlineStr"/>
       <c r="U13" t="inlineStr"/>
       <c r="V13" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1323,6 +1354,7 @@
       <c r="T14" t="inlineStr"/>
       <c r="U14" t="inlineStr"/>
       <c r="V14" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1372,39 +1404,42 @@
         <v>7</v>
       </c>
       <c r="M15" t="n">
+        <v>727</v>
+      </c>
+      <c r="N15" t="n">
         <v>11.1</v>
       </c>
-      <c r="N15" t="inlineStr">
+      <c r="O15" t="inlineStr">
         <is>
           <t>0.7</t>
         </is>
       </c>
-      <c r="O15" t="n">
+      <c r="P15" t="n">
         <v>72.79000000000001</v>
       </c>
-      <c r="P15" t="n">
+      <c r="Q15" t="n">
         <v>-56.1305</v>
       </c>
-      <c r="Q15" t="n">
+      <c r="R15" t="n">
         <v>69.2405</v>
       </c>
-      <c r="R15" t="n">
+      <c r="S15" t="n">
         <v>-51.0664</v>
       </c>
-      <c r="S15" t="inlineStr">
+      <c r="T15" t="inlineStr">
         <is>
           <t>Upernavik</t>
         </is>
       </c>
-      <c r="T15" t="inlineStr">
+      <c r="U15" t="inlineStr">
         <is>
           <t>Ilulissat</t>
         </is>
       </c>
-      <c r="U15" t="n">
+      <c r="V15" t="n">
         <v>140</v>
       </c>
-      <c r="V15" t="inlineStr">
+      <c r="W15" t="inlineStr">
         <is>
           <t>flight to SFJ via JUV</t>
         </is>
@@ -1458,39 +1493,42 @@
         <v>18</v>
       </c>
       <c r="M16" t="n">
+        <v>342</v>
+      </c>
+      <c r="N16" t="n">
         <v>13.1</v>
       </c>
-      <c r="N16" t="inlineStr">
+      <c r="O16" t="inlineStr">
         <is>
           <t>end of flying</t>
         </is>
       </c>
-      <c r="O16" t="n">
+      <c r="P16" t="n">
         <v>69.2405</v>
       </c>
-      <c r="P16" t="n">
+      <c r="Q16" t="n">
         <v>-51.0664</v>
       </c>
-      <c r="Q16" t="n">
+      <c r="R16" t="n">
         <v>67.0106</v>
       </c>
-      <c r="R16" t="n">
+      <c r="S16" t="n">
         <v>-50.711</v>
       </c>
-      <c r="S16" t="inlineStr">
+      <c r="T16" t="inlineStr">
         <is>
           <t>Ilulissat</t>
         </is>
       </c>
-      <c r="T16" t="inlineStr">
+      <c r="U16" t="inlineStr">
         <is>
           <t>Kangerlussuaq</t>
         </is>
       </c>
-      <c r="U16" t="n">
+      <c r="V16" t="n">
         <v>140</v>
       </c>
-      <c r="V16" t="inlineStr">
+      <c r="W16" t="inlineStr">
         <is>
           <t>refuel in JAV then end day in SFJ</t>
         </is>
@@ -1525,6 +1563,7 @@
       <c r="T17" t="inlineStr"/>
       <c r="U17" t="inlineStr"/>
       <c r="V17" t="inlineStr"/>
+      <c r="W17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1574,39 +1613,42 @@
         <v>14</v>
       </c>
       <c r="M18" t="n">
+        <v>9</v>
+      </c>
+      <c r="N18" t="n">
         <v>12.4</v>
       </c>
-      <c r="N18" t="inlineStr">
+      <c r="O18" t="inlineStr">
         <is>
           <t>end of flying</t>
         </is>
       </c>
-      <c r="O18" t="n">
+      <c r="P18" t="n">
         <v>67.0106</v>
       </c>
-      <c r="P18" t="n">
+      <c r="Q18" t="n">
         <v>-50.711</v>
       </c>
-      <c r="Q18" t="n">
+      <c r="R18" t="n">
         <v>63.7553</v>
       </c>
-      <c r="R18" t="n">
+      <c r="S18" t="n">
         <v>-68.5506</v>
       </c>
-      <c r="S18" t="inlineStr">
+      <c r="T18" t="inlineStr">
         <is>
           <t>Kangerlussuaq</t>
         </is>
       </c>
-      <c r="T18" t="inlineStr">
+      <c r="U18" t="inlineStr">
         <is>
           <t>Iqaluit</t>
         </is>
       </c>
-      <c r="U18" t="n">
+      <c r="V18" t="n">
         <v>140</v>
       </c>
-      <c r="V18" t="inlineStr">
+      <c r="W18" t="inlineStr">
         <is>
           <t>return to Canada</t>
         </is>
@@ -1641,6 +1683,7 @@
       <c r="T19" t="inlineStr"/>
       <c r="U19" t="inlineStr"/>
       <c r="V19" t="inlineStr"/>
+      <c r="W19" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
costing of crew and weather days and more detail to summary tables
</commit_message>
<xml_diff>
--- a/planning_info/NE_chartering_2021_Aug_Borek.xlsx
+++ b/planning_info/NE_chartering_2021_Aug_Borek.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W19"/>
+  <dimension ref="A1:W17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -883,31 +883,91 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>3. weather delay</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
-      <c r="T7" t="inlineStr"/>
-      <c r="U7" t="inlineStr"/>
-      <c r="V7" t="inlineStr"/>
-      <c r="W7" t="inlineStr"/>
+          <t>2021-08-10</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>4</v>
+      </c>
+      <c r="D7" t="n">
+        <v>9</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>EGP</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>NAE</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>150</v>
+      </c>
+      <c r="H7" t="n">
+        <v>3</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="K7" t="n">
+        <v>282</v>
+      </c>
+      <c r="L7" t="n">
+        <v>3</v>
+      </c>
+      <c r="M7" t="n">
+        <v>1118</v>
+      </c>
+      <c r="N7" t="n">
+        <v>10.1</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="P7" t="n">
+        <v>75.62479999999999</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>-35.9729</v>
+      </c>
+      <c r="R7" t="n">
+        <v>75</v>
+      </c>
+      <c r="S7" t="n">
+        <v>-29.9997</v>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>EGP</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>NASA-E</t>
+        </is>
+      </c>
+      <c r="V7" t="n">
+        <v>140</v>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>maintanance at NASA-E</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -928,12 +988,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
+          <t>NAE</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
           <t>EGP</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>NAE</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -951,16 +1011,16 @@
         <v>1.1</v>
       </c>
       <c r="K8" t="n">
-        <v>282</v>
+        <v>846</v>
       </c>
       <c r="L8" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="M8" t="n">
-        <v>1118</v>
+        <v>836</v>
       </c>
       <c r="N8" t="n">
-        <v>10.1</v>
+        <v>15.2</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -968,25 +1028,25 @@
         </is>
       </c>
       <c r="P8" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>-29.9997</v>
+      </c>
+      <c r="R8" t="n">
         <v>75.62479999999999</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="S8" t="n">
         <v>-35.9729</v>
       </c>
-      <c r="R8" t="n">
-        <v>75</v>
-      </c>
-      <c r="S8" t="n">
-        <v>-29.9997</v>
-      </c>
       <c r="T8" t="inlineStr">
         <is>
+          <t>NASA-E</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
           <t>EGP</t>
-        </is>
-      </c>
-      <c r="U8" t="inlineStr">
-        <is>
-          <t>NASA-E</t>
         </is>
       </c>
       <c r="V8" t="n">
@@ -994,129 +1054,129 @@
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>maintanance at NASA-E</t>
+          <t>return to EGP for overnight 2</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2021-08-10</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>4</v>
-      </c>
-      <c r="D9" t="n">
-        <v>9</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>NAE</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>EGP</t>
-        </is>
-      </c>
-      <c r="G9" t="n">
-        <v>150</v>
-      </c>
-      <c r="H9" t="n">
-        <v>3</v>
-      </c>
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>total fly time no taxi or circling</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="K9" t="n">
-        <v>846</v>
-      </c>
-      <c r="L9" t="n">
-        <v>9</v>
-      </c>
-      <c r="M9" t="n">
-        <v>836</v>
-      </c>
-      <c r="N9" t="n">
-        <v>15.2</v>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>4.0</t>
-        </is>
-      </c>
-      <c r="P9" t="n">
-        <v>75</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>-29.9997</v>
-      </c>
-      <c r="R9" t="n">
-        <v>75.62479999999999</v>
-      </c>
-      <c r="S9" t="n">
-        <v>-35.9729</v>
-      </c>
-      <c r="T9" t="inlineStr">
-        <is>
-          <t>NASA-E</t>
-        </is>
-      </c>
-      <c r="U9" t="inlineStr">
-        <is>
-          <t>EGP</t>
-        </is>
-      </c>
-      <c r="V9" t="n">
-        <v>140</v>
-      </c>
-      <c r="W9" t="inlineStr">
-        <is>
-          <t>return to EGP for overnight 2</t>
-        </is>
-      </c>
+        <v>1.4</v>
+      </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2021-08-11</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>5</v>
+      </c>
+      <c r="D10" t="n">
+        <v>9</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>EGP</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>NAU</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>150</v>
+      </c>
+      <c r="H10" t="n">
+        <v>3</v>
+      </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>total fly time no taxi or circling</t>
+          <t>239</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="inlineStr"/>
-      <c r="U10" t="inlineStr"/>
-      <c r="V10" t="inlineStr"/>
-      <c r="W10" t="inlineStr"/>
+        <v>2.1</v>
+      </c>
+      <c r="K10" t="n">
+        <v>684</v>
+      </c>
+      <c r="L10" t="n">
+        <v>7</v>
+      </c>
+      <c r="M10" t="n">
+        <v>716</v>
+      </c>
+      <c r="N10" t="n">
+        <v>11.1</v>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="P10" t="n">
+        <v>75.62479999999999</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>-35.9729</v>
+      </c>
+      <c r="R10" t="n">
+        <v>73.8419</v>
+      </c>
+      <c r="S10" t="n">
+        <v>-49.4983</v>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>EGP</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>NASA-U</t>
+        </is>
+      </c>
+      <c r="V10" t="n">
+        <v>140</v>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>crane maintanance at NASA-U</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1137,12 +1197,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>EGP</t>
+          <t>NAU</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>NAU</t>
+          <t>JUV</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -1153,49 +1213,49 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>239</t>
+          <t>131</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>2.1</v>
+        <v>1.3</v>
       </c>
       <c r="K11" t="n">
-        <v>684</v>
+        <v>1742</v>
       </c>
       <c r="L11" t="n">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="M11" t="n">
-        <v>716</v>
+        <v>342</v>
       </c>
       <c r="N11" t="n">
-        <v>11.1</v>
+        <v>16.4</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>end of flying</t>
         </is>
       </c>
       <c r="P11" t="n">
-        <v>75.62479999999999</v>
+        <v>73.8419</v>
       </c>
       <c r="Q11" t="n">
-        <v>-35.9729</v>
+        <v>-49.4983</v>
       </c>
       <c r="R11" t="n">
-        <v>73.8419</v>
+        <v>72.79000000000001</v>
       </c>
       <c r="S11" t="n">
-        <v>-49.4983</v>
+        <v>-56.1305</v>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>EGP</t>
+          <t>NASA-U</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>NASA-U</t>
+          <t>Upernavik</t>
         </is>
       </c>
       <c r="V11" t="n">
@@ -1203,273 +1263,275 @@
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>crane maintanance at NASA-U</t>
+          <t>return to coast. Upernavik</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2021-08-11</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>5</v>
-      </c>
-      <c r="D12" t="n">
-        <v>9</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>NAU</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>JUV</t>
-        </is>
-      </c>
-      <c r="G12" t="n">
-        <v>150</v>
-      </c>
-      <c r="H12" t="n">
-        <v>3</v>
-      </c>
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr">
         <is>
-          <t>131</t>
+          <t>total fly time no taxi or circling</t>
         </is>
       </c>
       <c r="J12" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="K12" t="n">
-        <v>1742</v>
-      </c>
-      <c r="L12" t="n">
-        <v>18</v>
-      </c>
-      <c r="M12" t="n">
-        <v>342</v>
-      </c>
-      <c r="N12" t="n">
-        <v>16.4</v>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>end of flying</t>
-        </is>
-      </c>
-      <c r="P12" t="n">
-        <v>73.8419</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>-49.4983</v>
-      </c>
-      <c r="R12" t="n">
-        <v>72.79000000000001</v>
-      </c>
-      <c r="S12" t="n">
-        <v>-56.1305</v>
-      </c>
-      <c r="T12" t="inlineStr">
-        <is>
-          <t>NASA-U</t>
-        </is>
-      </c>
-      <c r="U12" t="inlineStr">
-        <is>
-          <t>Upernavik</t>
-        </is>
-      </c>
-      <c r="V12" t="n">
-        <v>140</v>
-      </c>
-      <c r="W12" t="inlineStr">
-        <is>
-          <t>return to coast. Upernavik</t>
-        </is>
-      </c>
+        <v>2.6</v>
+      </c>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr"/>
+      <c r="R12" t="inlineStr"/>
+      <c r="S12" t="inlineStr"/>
+      <c r="T12" t="inlineStr"/>
+      <c r="U12" t="inlineStr"/>
+      <c r="V12" t="inlineStr"/>
+      <c r="W12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2021-08-13</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>7</v>
+      </c>
+      <c r="D13" t="n">
+        <v>9</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>JUV</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>JAV</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>150</v>
+      </c>
+      <c r="H13" t="n">
+        <v>3</v>
+      </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>total fly time no taxi or circling</t>
+          <t>236</t>
         </is>
       </c>
       <c r="J13" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="inlineStr"/>
-      <c r="S13" t="inlineStr"/>
-      <c r="T13" t="inlineStr"/>
-      <c r="U13" t="inlineStr"/>
-      <c r="V13" t="inlineStr"/>
-      <c r="W13" t="inlineStr"/>
+        <v>2.1</v>
+      </c>
+      <c r="K13" t="n">
+        <v>673</v>
+      </c>
+      <c r="L13" t="n">
+        <v>7</v>
+      </c>
+      <c r="M13" t="n">
+        <v>727</v>
+      </c>
+      <c r="N13" t="n">
+        <v>11.1</v>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>0.7</t>
+        </is>
+      </c>
+      <c r="P13" t="n">
+        <v>72.79000000000001</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>-56.1305</v>
+      </c>
+      <c r="R13" t="n">
+        <v>69.2405</v>
+      </c>
+      <c r="S13" t="n">
+        <v>-51.0664</v>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>Upernavik</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>Ilulissat</t>
+        </is>
+      </c>
+      <c r="V13" t="n">
+        <v>140</v>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>flight to SFJ via JUV</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>6. weather delay</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="inlineStr"/>
-      <c r="S14" t="inlineStr"/>
-      <c r="T14" t="inlineStr"/>
-      <c r="U14" t="inlineStr"/>
-      <c r="V14" t="inlineStr"/>
-      <c r="W14" t="inlineStr"/>
+          <t>2021-08-13</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>7</v>
+      </c>
+      <c r="D14" t="n">
+        <v>9</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>JAV</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>SFJ</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>150</v>
+      </c>
+      <c r="H14" t="n">
+        <v>3</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>135</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="K14" t="n">
+        <v>1731</v>
+      </c>
+      <c r="L14" t="n">
+        <v>18</v>
+      </c>
+      <c r="M14" t="n">
+        <v>342</v>
+      </c>
+      <c r="N14" t="n">
+        <v>13.1</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>end of flying</t>
+        </is>
+      </c>
+      <c r="P14" t="n">
+        <v>69.2405</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>-51.0664</v>
+      </c>
+      <c r="R14" t="n">
+        <v>67.0106</v>
+      </c>
+      <c r="S14" t="n">
+        <v>-50.711</v>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>Ilulissat</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>Kangerlussuaq</t>
+        </is>
+      </c>
+      <c r="V14" t="n">
+        <v>140</v>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>refuel in JAV then end day in SFJ</t>
+        </is>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2021-08-13</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>7</v>
-      </c>
-      <c r="D15" t="n">
-        <v>9</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>JUV</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>JAV</t>
-        </is>
-      </c>
-      <c r="G15" t="n">
-        <v>150</v>
-      </c>
-      <c r="H15" t="n">
-        <v>3</v>
-      </c>
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr">
         <is>
-          <t>236</t>
+          <t>total fly time no taxi or circling</t>
         </is>
       </c>
       <c r="J15" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="K15" t="n">
-        <v>673</v>
-      </c>
-      <c r="L15" t="n">
-        <v>7</v>
-      </c>
-      <c r="M15" t="n">
-        <v>727</v>
-      </c>
-      <c r="N15" t="n">
-        <v>11.1</v>
-      </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>0.7</t>
-        </is>
-      </c>
-      <c r="P15" t="n">
-        <v>72.79000000000001</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>-56.1305</v>
-      </c>
-      <c r="R15" t="n">
-        <v>69.2405</v>
-      </c>
-      <c r="S15" t="n">
-        <v>-51.0664</v>
-      </c>
-      <c r="T15" t="inlineStr">
-        <is>
-          <t>Upernavik</t>
-        </is>
-      </c>
-      <c r="U15" t="inlineStr">
-        <is>
-          <t>Ilulissat</t>
-        </is>
-      </c>
-      <c r="V15" t="n">
-        <v>140</v>
-      </c>
-      <c r="W15" t="inlineStr">
-        <is>
-          <t>flight to SFJ via JUV</t>
-        </is>
-      </c>
+        <v>2.6</v>
+      </c>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr"/>
+      <c r="Q15" t="inlineStr"/>
+      <c r="R15" t="inlineStr"/>
+      <c r="S15" t="inlineStr"/>
+      <c r="T15" t="inlineStr"/>
+      <c r="U15" t="inlineStr"/>
+      <c r="V15" t="inlineStr"/>
+      <c r="W15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2021-08-13</t>
+          <t>2021-08-14</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D16" t="n">
-        <v>9</v>
+        <v>8.5</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>JAV</t>
+          <t>SFJ</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>SFJ</t>
+          <t>IKA</t>
         </is>
       </c>
       <c r="G16" t="n">
@@ -1480,23 +1542,23 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>487</t>
         </is>
       </c>
       <c r="J16" t="n">
-        <v>1.4</v>
+        <v>3.9</v>
       </c>
       <c r="K16" t="n">
-        <v>1731</v>
+        <v>1391</v>
       </c>
       <c r="L16" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="M16" t="n">
-        <v>342</v>
+        <v>9</v>
       </c>
       <c r="N16" t="n">
-        <v>13.1</v>
+        <v>12.4</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1504,25 +1566,25 @@
         </is>
       </c>
       <c r="P16" t="n">
-        <v>69.2405</v>
+        <v>67.0106</v>
       </c>
       <c r="Q16" t="n">
-        <v>-51.0664</v>
+        <v>-50.711</v>
       </c>
       <c r="R16" t="n">
-        <v>67.0106</v>
+        <v>63.7553</v>
       </c>
       <c r="S16" t="n">
-        <v>-50.711</v>
+        <v>-68.5506</v>
       </c>
       <c r="T16" t="inlineStr">
         <is>
-          <t>Ilulissat</t>
+          <t>Kangerlussuaq</t>
         </is>
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>Kangerlussuaq</t>
+          <t>Iqaluit</t>
         </is>
       </c>
       <c r="V16" t="n">
@@ -1530,7 +1592,7 @@
       </c>
       <c r="W16" t="inlineStr">
         <is>
-          <t>refuel in JAV then end day in SFJ</t>
+          <t>return to Canada</t>
         </is>
       </c>
     </row>
@@ -1549,7 +1611,7 @@
         </is>
       </c>
       <c r="J17" t="n">
-        <v>2.6</v>
+        <v>3.5</v>
       </c>
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr"/>
@@ -1565,126 +1627,6 @@
       <c r="V17" t="inlineStr"/>
       <c r="W17" t="inlineStr"/>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>2021-08-14</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Saturday</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>8</v>
-      </c>
-      <c r="D18" t="n">
-        <v>8.5</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>SFJ</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>IKA</t>
-        </is>
-      </c>
-      <c r="G18" t="n">
-        <v>150</v>
-      </c>
-      <c r="H18" t="n">
-        <v>3</v>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>487</t>
-        </is>
-      </c>
-      <c r="J18" t="n">
-        <v>3.9</v>
-      </c>
-      <c r="K18" t="n">
-        <v>1391</v>
-      </c>
-      <c r="L18" t="n">
-        <v>14</v>
-      </c>
-      <c r="M18" t="n">
-        <v>9</v>
-      </c>
-      <c r="N18" t="n">
-        <v>12.4</v>
-      </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>end of flying</t>
-        </is>
-      </c>
-      <c r="P18" t="n">
-        <v>67.0106</v>
-      </c>
-      <c r="Q18" t="n">
-        <v>-50.711</v>
-      </c>
-      <c r="R18" t="n">
-        <v>63.7553</v>
-      </c>
-      <c r="S18" t="n">
-        <v>-68.5506</v>
-      </c>
-      <c r="T18" t="inlineStr">
-        <is>
-          <t>Kangerlussuaq</t>
-        </is>
-      </c>
-      <c r="U18" t="inlineStr">
-        <is>
-          <t>Iqaluit</t>
-        </is>
-      </c>
-      <c r="V18" t="n">
-        <v>140</v>
-      </c>
-      <c r="W18" t="inlineStr">
-        <is>
-          <t>return to Canada</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr"/>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>total fly time no taxi or circling</t>
-        </is>
-      </c>
-      <c r="J19" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr"/>
-      <c r="O19" t="inlineStr"/>
-      <c r="P19" t="inlineStr"/>
-      <c r="Q19" t="inlineStr"/>
-      <c r="R19" t="inlineStr"/>
-      <c r="S19" t="inlineStr"/>
-      <c r="T19" t="inlineStr"/>
-      <c r="U19" t="inlineStr"/>
-      <c r="V19" t="inlineStr"/>
-      <c r="W19" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>